<commit_message>
incorporated new version of the DrillingEquipment spreadsheet
</commit_message>
<xml_diff>
--- a/docs/vocabulary_development/definitions/DrillingEquipment.xlsx
+++ b/docs/vocabulary_development/definitions/DrillingEquipment.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Digital Oilfield\OSDU - DWIS\Contextual Data\Working Document\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DWIS\DDHub-Semantic-Interoperability\docs\vocabulary_development\definitions\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D006A7E-3DC8-40A9-B888-540554C75D4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18432" windowHeight="5112"/>
+    <workbookView xWindow="-27330" yWindow="1470" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FreeMind Sheet" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="435">
   <si>
     <t>&lt;equipment&gt;</t>
   </si>
@@ -1321,13 +1322,16 @@
   </si>
   <si>
     <t>Three Way Manifold</t>
+  </si>
+  <si>
+    <t>Three Way Valve</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1461,11 +1465,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1823,7 +1822,7 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1853,7 +1852,7 @@
     <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="attribute_cell" xfId="42"/>
+    <cellStyle name="attribute_cell" xfId="42" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
     <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
@@ -2148,2232 +2147,2237 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G442"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G443"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="A422" workbookViewId="0">
+      <selection activeCell="D442" sqref="D442"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E31" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E34" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E35" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E36" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E37" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E38" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E39" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E40" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E42" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E43" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:6" x14ac:dyDescent="0.25">
       <c r="F44" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:6" x14ac:dyDescent="0.25">
       <c r="F45" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:6" x14ac:dyDescent="0.25">
       <c r="F46" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:6" x14ac:dyDescent="0.25">
       <c r="F47" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D49" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D50" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D51" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E52" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E53" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E54" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D55" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E56" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E57" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E58" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E59" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D60" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D61" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D62" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E63" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F64" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D65" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D66" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D67" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D68" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E69" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E70" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E71" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D72" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D73" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D74" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D75" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E76" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E77" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E78" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D79" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D80" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C81" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D82" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E83" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="3:7" x14ac:dyDescent="0.25">
       <c r="F84" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="3:7" x14ac:dyDescent="0.25">
       <c r="F85" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="3:7" x14ac:dyDescent="0.25">
       <c r="F86" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="3:7" x14ac:dyDescent="0.25">
       <c r="F87" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="3:7" x14ac:dyDescent="0.25">
       <c r="F88" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="3:7" x14ac:dyDescent="0.25">
       <c r="G89" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="3:7" x14ac:dyDescent="0.25">
       <c r="G90" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E91" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E92" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E93" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E94" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E95" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D96" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D97" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D98" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D99" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D100" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E101" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E102" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E103" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E104" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E105" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E106" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E107" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="108" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D108" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="109" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E109" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E110" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="111" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E111" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="112" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E112" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="113" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E113" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="114" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E114" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="115" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E115" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="116" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="116" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E116" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="117" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="117" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E117" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="118" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="118" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E118" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="119" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="119" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D119" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="120" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="120" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E120" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="121" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="121" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E121" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="122" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F122" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="123" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="123" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F123" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="124" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="124" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E124" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="125" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="125" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D125" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="126" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="126" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D126" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="127" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="127" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E127" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="128" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="128" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E128" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="129" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="129" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D129" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="130" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="130" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D130" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="131" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="131" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D131" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="132" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="132" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E132" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="133" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="133" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E133" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="134" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="134" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E134" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="135" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="135" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E135" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="136" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="136" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E136" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="137" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="137" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C137" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="138" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="138" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D138" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="139" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="139" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E139" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="140" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="140" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E140" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="141" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="141" spans="3:6" x14ac:dyDescent="0.25">
       <c r="F141" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="142" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="142" spans="3:6" x14ac:dyDescent="0.25">
       <c r="F142" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="143" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="143" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E143" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="144" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="144" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D144" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="145" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="145" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D145" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="146" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="146" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D146" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="147" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="147" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D147" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="148" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="148" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D148" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="149" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="149" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D149" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="150" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="150" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D150" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="151" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="151" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D151" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="152" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="152" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D152" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="153" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="153" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D153" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="154" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="154" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D154" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="155" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="155" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D155" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="156" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="156" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D156" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="157" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="157" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D157" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="158" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="158" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D158" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="159" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="159" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E159" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="160" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="160" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E160" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="161" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="161" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D161" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="162" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="162" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D162" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="163" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="163" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D163" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="164" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="164" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D164" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="165" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="165" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C165" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="166" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="166" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D166" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="167" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="167" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E167" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="168" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="168" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E168" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="169" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="169" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E169" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="170" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="170" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E170" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="171" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="171" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D171" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="172" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="172" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E172" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="173" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="173" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E173" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="174" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="174" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E174" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="175" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="175" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E175" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="176" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="176" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E176" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="177" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="177" spans="3:6" x14ac:dyDescent="0.25">
       <c r="F177" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="178" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="178" spans="3:6" x14ac:dyDescent="0.25">
       <c r="F178" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="179" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="179" spans="3:6" x14ac:dyDescent="0.25">
       <c r="F179" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="180" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="180" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E180" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="181" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="181" spans="3:6" x14ac:dyDescent="0.25">
       <c r="F181" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="182" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="182" spans="3:6" x14ac:dyDescent="0.25">
       <c r="F182" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="183" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="183" spans="3:6" x14ac:dyDescent="0.25">
       <c r="F183" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="184" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="184" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E184" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="185" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="185" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E185" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="186" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="186" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E186" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="187" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="187" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E187" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="188" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="188" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E188" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="189" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="189" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E189" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="190" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="190" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C190" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="191" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="191" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D191" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="192" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="192" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D192" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="193" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="193" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D193" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="194" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="194" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D194" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="195" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="195" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D195" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="196" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="196" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D196" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="197" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="197" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D197" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="198" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="198" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D198" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="199" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="199" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D199" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="200" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="200" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C200" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="201" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="201" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D201" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="202" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="202" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D202" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="203" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="203" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D203" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="204" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="204" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D204" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="205" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="205" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D205" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="206" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="206" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C206" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="207" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="207" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D207" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="208" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="208" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D208" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="209" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="209" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C209" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="210" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="210" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D210" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="211" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="211" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C211" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="212" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="212" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D212" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="213" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="213" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D213" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="214" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="214" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D214" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="215" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="215" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D215" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="216" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="216" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B216" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="217" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="217" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C217" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="218" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="218" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D218" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="219" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="219" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D219" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="220" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="220" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D220" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="221" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="221" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D221" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="222" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="222" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D222" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="223" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="223" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D223" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="224" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="224" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D224" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="225" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="225" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D225" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="226" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="226" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D226" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="227" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="227" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E227" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="228" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="228" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F228" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="229" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="229" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F229" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="230" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="230" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F230" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="231" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="231" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F231" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="232" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="232" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F232" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="233" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="233" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E233" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="234" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="234" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F234" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="235" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="235" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F235" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="236" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="236" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F236" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="237" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="237" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F237" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="238" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="238" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E238" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="239" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="239" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E239" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="240" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="240" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E240" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="241" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="241" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E241" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="242" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="242" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E242" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="243" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="243" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E243" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="244" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="244" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D244" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="245" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="245" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E245" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="246" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="246" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E246" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="247" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="247" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E247" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="248" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="248" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D248" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="249" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="249" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E249" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="250" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="250" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E250" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="251" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="251" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E251" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="252" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="252" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E252" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="253" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="253" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E253" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="254" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="254" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E254" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="255" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="255" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E255" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="256" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="256" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E256" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="257" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="257" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E257" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="258" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="258" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E258" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="259" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="259" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E259" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="260" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="260" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E260" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="261" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="261" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E261" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="262" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="262" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E262" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="263" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="263" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E263" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="264" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="264" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E264" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="265" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="265" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E265" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="266" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="266" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E266" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="267" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="267" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E267" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="268" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="268" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E268" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="269" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="269" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E269" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="270" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="270" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C270" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="271" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="271" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D271" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="272" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="272" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D272" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="273" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="273" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D273" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="274" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="274" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D274" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="275" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="275" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D275" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="276" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="276" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D276" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="277" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="277" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E277" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="278" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="278" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E278" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="279" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="279" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E279" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="280" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="280" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E280" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="281" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="281" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E281" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="282" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="282" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E282" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="283" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="283" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C283" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="284" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="284" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C284" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="285" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="285" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C285" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="286" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="286" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C286" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="287" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="287" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C287" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="288" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="288" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D288" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="289" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="289" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D289" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="290" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="290" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D290" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="291" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="291" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D291" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="292" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="292" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B292" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="293" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="293" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C293" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="294" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="294" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D294" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="295" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="295" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E295" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="296" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="296" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F296" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="297" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="297" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G297" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="298" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="298" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G298" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="299" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="299" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F299" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="300" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="300" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G300" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="301" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="301" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G301" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="302" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="302" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G302" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="303" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="303" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G303" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="304" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="304" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F304" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="305" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="305" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F305" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="306" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="306" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E306" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="307" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="307" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D307" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="308" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="308" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E308" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="309" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="309" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E309" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="310" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="310" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E310" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="311" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="311" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E311" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="312" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="312" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E312" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="313" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="313" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E313" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="314" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="314" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D314" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="315" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="315" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E315" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="316" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="316" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E316" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="317" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="317" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D317" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="318" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="318" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E318" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="319" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="319" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E319" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="320" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="320" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D320" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="321" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="321" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E321" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="322" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="322" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E322" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="323" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="323" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E323" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="324" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="324" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E324" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="325" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="325" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E325" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="326" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="326" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E326" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="327" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="327" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D327" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="328" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="328" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D328" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="329" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="329" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E329" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="330" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="330" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E330" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="331" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="331" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E331" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="332" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="332" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D332" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="333" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="333" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D333" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="334" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="334" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D334" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="335" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="335" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E335" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="336" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="336" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E336" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="337" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="337" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E337" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="338" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="338" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E338" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="339" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="339" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E339" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="340" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="340" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D340" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="341" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="341" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E341" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="342" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="342" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D342" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="343" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="343" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E343" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="344" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="344" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D344" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="345" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="345" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D345" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="346" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="346" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D346" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="347" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="347" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E347" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="348" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="348" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E348" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="349" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="349" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E349" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="350" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="350" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D350" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="351" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="351" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D351" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="352" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="352" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E352" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="353" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="353" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E353" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="354" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="354" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E354" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="355" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="355" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D355" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="356" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="356" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C356" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="357" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="357" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D357" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="358" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="358" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E358" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="359" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="359" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E359" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="360" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="360" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E360" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="361" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="361" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E361" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="362" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="362" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E362" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="363" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="363" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E363" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="364" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="364" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E364" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="365" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="365" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E365" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="366" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="366" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E366" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="367" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="367" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E367" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="368" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="368" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E368" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="369" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="369" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D369" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="370" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="370" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D370" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="371" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="371" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D371" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="372" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="372" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D372" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="373" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="373" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D373" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="374" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="374" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D374" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="375" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="375" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D375" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="376" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="376" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D376" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="377" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="377" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D377" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="378" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="378" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E378" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="379" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="379" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E379" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="380" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="380" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E380" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="381" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="381" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D381" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="382" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="382" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D382" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="383" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="383" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D383" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="384" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="384" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D384" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="385" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="385" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D385" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="386" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="386" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C386" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="387" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="387" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D387" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="388" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="388" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E388" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="389" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="389" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E389" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="390" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="390" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E390" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="391" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="391" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E391" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="392" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="392" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E392" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="393" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="393" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E393" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="394" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="394" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D394" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="395" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="395" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E395" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="396" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="396" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E396" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="397" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="397" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E397" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="398" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="398" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D398" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="399" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="399" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E399" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="400" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="400" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E400" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="401" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="401" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E401" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="402" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="402" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E402" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="403" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="403" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E403" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="404" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="404" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E404" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="405" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="405" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E405" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="406" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="406" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E406" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="407" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="407" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E407" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="408" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="408" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D408" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="409" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="409" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E409" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="410" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="410" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E410" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="411" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="411" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E411" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="412" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="412" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D412" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="413" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="413" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E413" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="414" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="414" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E414" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="415" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="415" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E415" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="416" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="416" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E416" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="417" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="417" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E417" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="418" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="418" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E418" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="419" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="419" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E419" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="420" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="420" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E420" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="421" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="421" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E421" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="422" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="422" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E422" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="423" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="423" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E423" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="424" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="424" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E424" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="425" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="425" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E425" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="426" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="426" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E426" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="427" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="427" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E427" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="428" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="428" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E428" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="429" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="429" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E429" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="430" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="430" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B430" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="431" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="431" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C431" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="432" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="432" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C432" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="433" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="433" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C433" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="434" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="434" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C434" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="435" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="435" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C435" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="436" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="436" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D436" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="437" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="437" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C437" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="438" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="438" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C438" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="439" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="439" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C439" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="440" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="440" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B440" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="441" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="441" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C441" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="442" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="442" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C442" t="s">
         <v>433</v>
+      </c>
+    </row>
+    <row r="443" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C443" t="s">
+        <v>434</v>
       </c>
     </row>
   </sheetData>

</xml_diff>